<commit_message>
Added support for suite level in excel and modify readme document
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/FrameworkSheet.xlsx
+++ b/src/test/resources/ExcelData/FrameworkSheet.xlsx
@@ -5,67 +5,74 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TestSuite" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="googleplace" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
-  <si>
-    <t>Select Base URL</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+  <si>
+    <t>Test Sheet Name</t>
+  </si>
+  <si>
+    <t>Test Mode</t>
+  </si>
+  <si>
+    <t>googleplace</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Test Base URL</t>
   </si>
   <si>
     <t>https://maps.googleapis.com</t>
   </si>
   <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>TFNameAndDesc</t>
-  </si>
-  <si>
-    <t>TCName</t>
-  </si>
-  <si>
-    <t>Api Type</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Input Json</t>
-  </si>
-  <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>Expected Status code</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>Method and json path</t>
-  </si>
-  <si>
-    <t>Assert Response</t>
+    <t>Test Id</t>
+  </si>
+  <si>
+    <t>Test Flow Name</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Test Api Type</t>
+  </si>
+  <si>
+    <t>Test Url</t>
+  </si>
+  <si>
+    <t>Test Input Json</t>
+  </si>
+  <si>
+    <t>Test Headers</t>
+  </si>
+  <si>
+    <t>Test Schema Name</t>
+  </si>
+  <si>
+    <t>Test Expected Status Code</t>
+  </si>
+  <si>
+    <t>Test Parameters</t>
+  </si>
+  <si>
+    <t>Test Method and json path</t>
+  </si>
+  <si>
+    <t>Test Assert Response</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Search Place</t>
@@ -118,8 +125,8 @@
   <si>
     <t>{
   "location": {
-    "lat": #1.lat#,
-    "lng": #1.lng#
+    "lat": #googleplace.1.lat#,
+    "lng": #googleplace.1.lng#
   },
   "accuracy": 50,
   "name": "Test",
@@ -128,45 +135,46 @@
   "types": ["shoe_store"],
   "website": "http://www.google.com.au/",
   "language": "en-AU"
+}
+      </t>
+  </si>
+  <si>
+    <t>addplace.json</t>
+  </si>
+  <si>
+    <t>?key=$$$$$$$</t>
+  </si>
+  <si>
+    <t>extractString:$.place_id;extractString:$.scope</t>
+  </si>
+  <si>
+    <t>#googleplace.3.scope#,APP</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Delete Place</t>
+  </si>
+  <si>
+    <t>deletePlace</t>
+  </si>
+  <si>
+    <t>/maps/api/place/delete/json</t>
+  </si>
+  <si>
+    <t>{
+  "place_id": "#googleplace.3.place_id#"
 }</t>
   </si>
   <si>
-    <t>addplace.json</t>
-  </si>
-  <si>
-    <t>?key=$$$$$$$</t>
-  </si>
-  <si>
-    <t>extractString:$.place_id;extractString:$.scope</t>
-  </si>
-  <si>
-    <t>#3.scope#,APP</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Delete Place</t>
-  </si>
-  <si>
-    <t>deletePlace</t>
-  </si>
-  <si>
-    <t>/maps/api/place/delete/json</t>
-  </si>
-  <si>
-    <t>{
-  "place_id": "#3.place_id#"
-}</t>
-  </si>
-  <si>
     <t>deleteplace.json</t>
   </si>
   <si>
     <t>extractString:$.status</t>
   </si>
   <si>
-    <t>#4.status#,OK</t>
+    <t>#googleplace.4.status#,OK</t>
   </si>
 </sst>
 </file>
@@ -200,6 +208,18 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Times New Roman"/>
@@ -218,18 +238,6 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -274,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -291,6 +299,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right/>
       <top style="thin"/>
       <bottom/>
@@ -322,28 +337,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,11 +366,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,11 +394,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,7 +406,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,248 +487,290 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.4285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.0969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="36.5357142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.6479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.8469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.2908163265306"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="J3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="K3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="L3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="6" t="s">
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="206.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="K4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="L4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="237.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="J5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="82.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="L5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="M5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="11" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="90.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="6" t="s">
+      <c r="E6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="J6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Added support for skip test if dynamic value not present, Modify readme document, Modify the size for the response value,Added support for getting values from list and improves the excel logic for reading
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/FrameworkSheet.xlsx
+++ b/src/test/resources/ExcelData/FrameworkSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="435" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Test Sheet Name</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Test Assert Response</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Search Place</t>
   </si>
   <si>
@@ -90,25 +87,16 @@
     <t>searchplace.json</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>?query=restaurants in pashan&amp;key=$$$$$$$</t>
   </si>
   <si>
     <t>extractNumber:$.results[0].geometry.location.lat;extractNumber:$.results[0].geometry.location.lng</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>serachPlaceBaner</t>
   </si>
   <si>
     <t>?query=restaurants in baner&amp;key=$$$$$$$</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>Add Place</t>
@@ -135,8 +123,7 @@
   "types": ["shoe_store"],
   "website": "http://www.google.com.au/",
   "language": "en-AU"
-}
-      </t>
+}</t>
   </si>
   <si>
     <t>addplace.json</t>
@@ -149,9 +136,6 @@
   </si>
   <si>
     <t>#googleplace.3.scope#,APP</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>Delete Place</t>
@@ -532,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -614,147 +598,147 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
+      <c r="A3" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="13"/>
       <c r="I3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="M3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
+      <c r="A4" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="13"/>
       <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="237.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>30</v>
+      <c r="A5" s="6" t="n">
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>200</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
+      <c r="A6" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>200</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>